<commit_message>
plots of rain by year now include 2-year design storm
</commit_message>
<xml_diff>
--- a/excel/HLC_Average_Monthly_Runoff_Adjusted.xlsx
+++ b/excel/HLC_Average_Monthly_Runoff_Adjusted.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\python\hlc_cuhp\excel\"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Subcatchment</t>
   </si>
@@ -133,6 +133,9 @@
   <si>
     <t>Totals</t>
   </si>
+  <si>
+    <t>Average Montly Runoff (ac-ft)</t>
+  </si>
 </sst>
 </file>
 
@@ -141,7 +144,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,16 +168,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -182,16 +207,124 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -256,10 +389,9 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Lines represent entrance points</a:t>
+              <a:rPr lang="en-US" sz="1260" baseline="0"/>
+              <a:t>Lines represent entrance points/subcatchments</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -315,9 +447,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -335,16 +467,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$K$3</c:f>
+              <c:f>Sheet1!$F$4:$L$4</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>4.5485994011400001E-2</c:v>
                 </c:pt>
@@ -362,6 +497,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.7514082247099999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -390,9 +528,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -410,16 +548,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$K$4</c:f>
+              <c:f>Sheet1!$F$5:$L$5</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2.93818091747</c:v>
                 </c:pt>
@@ -437,6 +578,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.7772800875799999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -465,9 +609,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -485,16 +629,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$5:$K$5</c:f>
+              <c:f>Sheet1!$F$6:$L$6</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>4.5584652325099997</c:v>
                 </c:pt>
@@ -512,6 +659,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.75737598032</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -540,9 +690,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -560,16 +710,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$6:$K$6</c:f>
+              <c:f>Sheet1!$F$7:$L$7</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>6.6398275366599993E-2</c:v>
                 </c:pt>
@@ -587,6 +740,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.0163739392900001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -615,9 +771,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -635,16 +791,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$7:$K$7</c:f>
+              <c:f>Sheet1!$F$8:$L$8</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.81176870228</c:v>
                 </c:pt>
@@ -662,6 +821,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.0959231334999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -690,9 +852,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -710,16 +872,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$8:$K$8</c:f>
+              <c:f>Sheet1!$F$9:$L$9</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>5.1533714709999998</c:v>
                 </c:pt>
@@ -737,6 +902,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.1172295908800001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -767,9 +935,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -787,16 +955,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$9:$K$9</c:f>
+              <c:f>Sheet1!$F$10:$L$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.82255476016200002</c:v>
                 </c:pt>
@@ -814,6 +985,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.49755622177199998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -844,9 +1018,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -864,16 +1038,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$10:$K$10</c:f>
+              <c:f>Sheet1!$F$11:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.76802290473</c:v>
                 </c:pt>
@@ -891,6 +1068,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.0694616809599999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -921,9 +1101,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -941,16 +1121,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$11:$K$11</c:f>
+              <c:f>Sheet1!$F$12:$L$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>4.1242356245299998</c:v>
                 </c:pt>
@@ -968,6 +1151,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.4947142663599999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -998,9 +1184,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -1018,16 +1204,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$12:$K$12</c:f>
+              <c:f>Sheet1!$F$13:$L$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.13849877789</c:v>
                 </c:pt>
@@ -1045,6 +1234,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.68866801075399997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1075,9 +1267,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -1095,16 +1287,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$13:$K$13</c:f>
+              <c:f>Sheet1!$F$14:$L$14</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.91352585422900001</c:v>
                 </c:pt>
@@ -1122,6 +1317,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.55258384551999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1152,9 +1350,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -1172,16 +1370,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$14:$K$14</c:f>
+              <c:f>Sheet1!$F$15:$L$15</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>9.2543191189700007</c:v>
                 </c:pt>
@@ -1199,6 +1400,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5.5978571627299996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1230,9 +1434,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -1250,16 +1454,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$15:$K$15</c:f>
+              <c:f>Sheet1!$F$16:$L$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>4.80775727459E-2</c:v>
                 </c:pt>
@@ -1277,6 +1484,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.90817056881E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1308,9 +1518,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -1328,16 +1538,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$16:$K$16</c:f>
+              <c:f>Sheet1!$F$17:$L$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.29672347742299998</c:v>
                 </c:pt>
@@ -1355,6 +1568,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.17948545128900001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1386,9 +1602,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -1406,16 +1622,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$17:$K$17</c:f>
+              <c:f>Sheet1!$F$18:$L$18</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>6.5711996053400001E-3</c:v>
                 </c:pt>
@@ -1433,6 +1652,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.9748615004099996E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1464,9 +1686,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -1484,16 +1706,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$18:$K$18</c:f>
+              <c:f>Sheet1!$F$19:$L$19</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2.3028684184800001</c:v>
                 </c:pt>
@@ -1511,6 +1736,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.3929850814</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1542,9 +1770,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -1562,16 +1790,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$19:$K$19</c:f>
+              <c:f>Sheet1!$F$20:$L$20</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.44992271947099999</c:v>
                 </c:pt>
@@ -1589,6 +1820,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.272154340637</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1620,9 +1854,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -1640,16 +1874,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$20:$K$20</c:f>
+              <c:f>Sheet1!$F$21:$L$21</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.6640229122500001</c:v>
                 </c:pt>
@@ -1667,6 +1904,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.0065529898500001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1697,9 +1937,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -1717,16 +1957,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$21:$K$21</c:f>
+              <c:f>Sheet1!$F$22:$L$22</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>14.137242987300001</c:v>
                 </c:pt>
@@ -1744,6 +1987,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>8.5514953504700006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1774,9 +2020,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -1794,16 +2040,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$22:$K$22</c:f>
+              <c:f>Sheet1!$F$23:$L$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>3.36500166636</c:v>
                 </c:pt>
@@ -1821,6 +2070,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.0354602471000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1851,9 +2103,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -1871,16 +2123,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$23:$K$23</c:f>
+              <c:f>Sheet1!$F$24:$L$24</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>6.0013167251599997E-2</c:v>
                 </c:pt>
@@ -1898,6 +2153,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.6301443016800002E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1928,9 +2186,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -1948,16 +2206,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$24:$K$24</c:f>
+              <c:f>Sheet1!$F$25:$L$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.107099039398</c:v>
                 </c:pt>
@@ -1975,6 +2236,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6.4783277635700007E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2005,9 +2269,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -2025,16 +2289,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$25:$K$25</c:f>
+              <c:f>Sheet1!$F$26:$L$26</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>5.8433857149499998E-3</c:v>
                 </c:pt>
@@ -2052,6 +2319,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.53461320692E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2082,9 +2352,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -2102,16 +2372,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$26:$K$26</c:f>
+              <c:f>Sheet1!$F$27:$L$27</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.04263085165</c:v>
                 </c:pt>
@@ -2129,6 +2402,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.63067833580900001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2160,9 +2436,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -2180,16 +2456,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$27:$K$27</c:f>
+              <c:f>Sheet1!$F$28:$L$28</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>14.422518612899999</c:v>
                 </c:pt>
@@ -2207,6 +2486,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>8.72405609572</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2238,9 +2520,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -2258,16 +2540,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$28:$K$28</c:f>
+              <c:f>Sheet1!$F$29:$L$29</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>12.916431923099999</c:v>
                 </c:pt>
@@ -2285,6 +2570,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>7.8130373535100004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2316,9 +2604,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$K$2</c:f>
+              <c:f>Sheet1!$F$3:$L$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>April</c:v>
                 </c:pt>
@@ -2336,16 +2624,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>October</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$29:$K$29</c:f>
+              <c:f>Sheet1!$F$30:$L$30</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>4.7495701723800003</c:v>
                 </c:pt>
@@ -2363,6 +2654,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.8729736966699999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3160,15 +3454,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>142874</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3489,10 +3783,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A2:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3504,74 +3799,46 @@
     <col min="6" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E2" s="3" t="s">
+    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="F2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="2">
-        <v>4.5485994011400001E-2</v>
-      </c>
-      <c r="G3" s="2">
-        <v>6.0636672075400001E-2</v>
-      </c>
-      <c r="H3" s="2">
-        <v>5.71925463621E-2</v>
-      </c>
-      <c r="I3" s="2">
-        <v>4.5609597256000001E-2</v>
-      </c>
-      <c r="J3" s="2">
-        <v>4.1085718503699999E-2</v>
-      </c>
-      <c r="K3" s="2">
-        <v>2.7514082247099999E-2</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0</v>
+      <c r="E3" s="11"/>
+      <c r="F3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3579,28 +3846,28 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="2">
-        <v>2.93818091747</v>
-      </c>
-      <c r="G4" s="2">
-        <v>3.11060581447</v>
-      </c>
-      <c r="H4" s="2">
-        <v>2.1727235551000001</v>
-      </c>
-      <c r="I4" s="2">
-        <v>2.9461651047499999</v>
-      </c>
-      <c r="J4" s="2">
-        <v>2.6539438504500001</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1.7772800875799999</v>
-      </c>
-      <c r="L4" s="2">
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="12">
+        <v>4.5485994011400001E-2</v>
+      </c>
+      <c r="G4" s="12">
+        <v>6.0636672075400001E-2</v>
+      </c>
+      <c r="H4" s="12">
+        <v>5.71925463621E-2</v>
+      </c>
+      <c r="I4" s="12">
+        <v>4.5609597256000001E-2</v>
+      </c>
+      <c r="J4" s="12">
+        <v>4.1085718503699999E-2</v>
+      </c>
+      <c r="K4" s="12">
+        <v>2.7514082247099999E-2</v>
+      </c>
+      <c r="L4" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3609,28 +3876,28 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="2">
-        <v>4.5584652325099997</v>
-      </c>
-      <c r="G5" s="2">
-        <v>4.7938207744000003</v>
-      </c>
-      <c r="H5" s="2">
-        <v>3.35902694425</v>
-      </c>
-      <c r="I5" s="2">
-        <v>4.5708523662899996</v>
-      </c>
-      <c r="J5" s="2">
-        <v>4.1174832698000001</v>
-      </c>
-      <c r="K5" s="2">
-        <v>2.75737598032</v>
-      </c>
-      <c r="L5" s="2">
+      <c r="E5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="12">
+        <v>2.93818091747</v>
+      </c>
+      <c r="G5" s="12">
+        <v>3.11060581447</v>
+      </c>
+      <c r="H5" s="12">
+        <v>2.1727235551000001</v>
+      </c>
+      <c r="I5" s="12">
+        <v>2.9461651047499999</v>
+      </c>
+      <c r="J5" s="12">
+        <v>2.6539438504500001</v>
+      </c>
+      <c r="K5" s="12">
+        <v>1.7772800875799999</v>
+      </c>
+      <c r="L5" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3639,28 +3906,28 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="2">
-        <v>6.6398275366599993E-2</v>
-      </c>
-      <c r="G6" s="2">
-        <v>9.7829896129000005E-2</v>
-      </c>
-      <c r="H6" s="2">
-        <v>9.8092813673500007E-2</v>
-      </c>
-      <c r="I6" s="2">
-        <v>6.6578705462700005E-2</v>
-      </c>
-      <c r="J6" s="2">
-        <v>5.9974963945200001E-2</v>
-      </c>
-      <c r="K6" s="2">
-        <v>4.0163739392900001E-2</v>
-      </c>
-      <c r="L6" s="2">
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="12">
+        <v>4.5584652325099997</v>
+      </c>
+      <c r="G6" s="12">
+        <v>4.7938207744000003</v>
+      </c>
+      <c r="H6" s="12">
+        <v>3.35902694425</v>
+      </c>
+      <c r="I6" s="12">
+        <v>4.5708523662899996</v>
+      </c>
+      <c r="J6" s="12">
+        <v>4.1174832698000001</v>
+      </c>
+      <c r="K6" s="12">
+        <v>2.75737598032</v>
+      </c>
+      <c r="L6" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3669,28 +3936,28 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1.81176870228</v>
-      </c>
-      <c r="G7" s="2">
-        <v>1.9289692865400001</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1.3624119860999999</v>
-      </c>
-      <c r="I7" s="2">
-        <v>1.8166919868</v>
-      </c>
-      <c r="J7" s="2">
-        <v>1.63649977347</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1.0959231334999999</v>
-      </c>
-      <c r="L7" s="2">
+      <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="12">
+        <v>6.6398275366599993E-2</v>
+      </c>
+      <c r="G7" s="12">
+        <v>9.7829896129000005E-2</v>
+      </c>
+      <c r="H7" s="12">
+        <v>9.8092813673500007E-2</v>
+      </c>
+      <c r="I7" s="12">
+        <v>6.6578705462700005E-2</v>
+      </c>
+      <c r="J7" s="12">
+        <v>5.9974963945200001E-2</v>
+      </c>
+      <c r="K7" s="12">
+        <v>4.0163739392900001E-2</v>
+      </c>
+      <c r="L7" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3699,28 +3966,28 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="2">
-        <v>5.1533714709999998</v>
-      </c>
-      <c r="G8" s="2">
-        <v>5.4402392390900003</v>
-      </c>
-      <c r="H8" s="2">
-        <v>3.8125623180899999</v>
-      </c>
-      <c r="I8" s="2">
-        <v>5.1673751978300002</v>
-      </c>
-      <c r="J8" s="2">
-        <v>4.65483879609</v>
-      </c>
-      <c r="K8" s="2">
-        <v>3.1172295908800001</v>
-      </c>
-      <c r="L8" s="2">
+      <c r="E8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="12">
+        <v>1.81176870228</v>
+      </c>
+      <c r="G8" s="12">
+        <v>1.9289692865400001</v>
+      </c>
+      <c r="H8" s="12">
+        <v>1.3624119860999999</v>
+      </c>
+      <c r="I8" s="12">
+        <v>1.8166919868</v>
+      </c>
+      <c r="J8" s="12">
+        <v>1.63649977347</v>
+      </c>
+      <c r="K8" s="12">
+        <v>1.0959231334999999</v>
+      </c>
+      <c r="L8" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3729,28 +3996,28 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.82255476016200002</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.86502362006099998</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0.64587759420099999</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0.82478996331400001</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0.74298152792899996</v>
-      </c>
-      <c r="K9" s="2">
-        <v>0.49755622177199998</v>
-      </c>
-      <c r="L9" s="2">
+      <c r="E9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="12">
+        <v>5.1533714709999998</v>
+      </c>
+      <c r="G9" s="12">
+        <v>5.4402392390900003</v>
+      </c>
+      <c r="H9" s="12">
+        <v>3.8125623180899999</v>
+      </c>
+      <c r="I9" s="12">
+        <v>5.1673751978300002</v>
+      </c>
+      <c r="J9" s="12">
+        <v>4.65483879609</v>
+      </c>
+      <c r="K9" s="12">
+        <v>3.1172295908800001</v>
+      </c>
+      <c r="L9" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3759,28 +4026,28 @@
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1.76802290473</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1.85930669601</v>
-      </c>
-      <c r="H10" s="2">
-        <v>1.3473669962999999</v>
-      </c>
-      <c r="I10" s="2">
-        <v>1.7728273148</v>
-      </c>
-      <c r="J10" s="2">
-        <v>1.59698590634</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1.0694616809599999</v>
-      </c>
-      <c r="L10" s="2">
+      <c r="E10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0.82255476016200002</v>
+      </c>
+      <c r="G10" s="12">
+        <v>0.86502362006099998</v>
+      </c>
+      <c r="H10" s="12">
+        <v>0.64587759420099999</v>
+      </c>
+      <c r="I10" s="12">
+        <v>0.82478996331400001</v>
+      </c>
+      <c r="J10" s="12">
+        <v>0.74298152792899996</v>
+      </c>
+      <c r="K10" s="12">
+        <v>0.49755622177199998</v>
+      </c>
+      <c r="L10" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3789,28 +4056,28 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="2">
-        <v>4.1242356245299998</v>
-      </c>
-      <c r="G11" s="2">
-        <v>4.3371717029700001</v>
-      </c>
-      <c r="H11" s="2">
-        <v>3.0202852664900002</v>
-      </c>
-      <c r="I11" s="2">
-        <v>4.1354427865499996</v>
-      </c>
-      <c r="J11" s="2">
-        <v>3.7252606565000002</v>
-      </c>
-      <c r="K11" s="2">
-        <v>2.4947142663599999</v>
-      </c>
-      <c r="L11" s="2">
+      <c r="E11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="12">
+        <v>1.76802290473</v>
+      </c>
+      <c r="G11" s="12">
+        <v>1.85930669601</v>
+      </c>
+      <c r="H11" s="12">
+        <v>1.3473669962999999</v>
+      </c>
+      <c r="I11" s="12">
+        <v>1.7728273148</v>
+      </c>
+      <c r="J11" s="12">
+        <v>1.59698590634</v>
+      </c>
+      <c r="K11" s="12">
+        <v>1.0694616809599999</v>
+      </c>
+      <c r="L11" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3819,28 +4086,28 @@
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1.13849877789</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1.2359942691500001</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0.90081503519799999</v>
-      </c>
-      <c r="I12" s="2">
-        <v>1.14159252457</v>
-      </c>
-      <c r="J12" s="2">
-        <v>1.02836139611</v>
-      </c>
-      <c r="K12" s="2">
-        <v>0.68866801075399997</v>
-      </c>
-      <c r="L12" s="2">
+      <c r="E12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="12">
+        <v>4.1242356245299998</v>
+      </c>
+      <c r="G12" s="12">
+        <v>4.3371717029700001</v>
+      </c>
+      <c r="H12" s="12">
+        <v>3.0202852664900002</v>
+      </c>
+      <c r="I12" s="12">
+        <v>4.1354427865499996</v>
+      </c>
+      <c r="J12" s="12">
+        <v>3.7252606565000002</v>
+      </c>
+      <c r="K12" s="12">
+        <v>2.4947142663599999</v>
+      </c>
+      <c r="L12" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3849,28 +4116,28 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0.91352585422900001</v>
-      </c>
-      <c r="G13" s="2">
-        <v>1.0686388898100001</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0.85439703176100001</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0.91600826144199998</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0.82515215746100001</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0.55258384551999995</v>
-      </c>
-      <c r="L13" s="2">
+      <c r="E13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="12">
+        <v>1.13849877789</v>
+      </c>
+      <c r="G13" s="12">
+        <v>1.2359942691500001</v>
+      </c>
+      <c r="H13" s="12">
+        <v>0.90081503519799999</v>
+      </c>
+      <c r="I13" s="12">
+        <v>1.14159252457</v>
+      </c>
+      <c r="J13" s="12">
+        <v>1.02836139611</v>
+      </c>
+      <c r="K13" s="12">
+        <v>0.68866801075399997</v>
+      </c>
+      <c r="L13" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3879,28 +4146,28 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="2">
-        <v>9.2543191189700007</v>
-      </c>
-      <c r="G14" s="2">
-        <v>9.8652577736799998</v>
-      </c>
-      <c r="H14" s="2">
-        <v>6.9642893628399998</v>
-      </c>
-      <c r="I14" s="2">
-        <v>9.2794667252699998</v>
-      </c>
-      <c r="J14" s="2">
-        <v>8.3590643346399993</v>
-      </c>
-      <c r="K14" s="2">
-        <v>5.5978571627299996</v>
-      </c>
-      <c r="L14" s="2">
+      <c r="E14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0.91352585422900001</v>
+      </c>
+      <c r="G14" s="12">
+        <v>1.0686388898100001</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0.85439703176100001</v>
+      </c>
+      <c r="I14" s="12">
+        <v>0.91600826144199998</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0.82515215746100001</v>
+      </c>
+      <c r="K14" s="12">
+        <v>0.55258384551999995</v>
+      </c>
+      <c r="L14" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3909,28 +4176,28 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="2">
-        <v>4.80775727459E-2</v>
-      </c>
-      <c r="G15" s="2">
-        <v>6.3433137419000002E-2</v>
-      </c>
-      <c r="H15" s="2">
-        <v>5.8545778175500003E-2</v>
-      </c>
-      <c r="I15" s="2">
-        <v>4.8208218323999998E-2</v>
-      </c>
-      <c r="J15" s="2">
-        <v>4.3426590165000001E-2</v>
-      </c>
-      <c r="K15" s="2">
-        <v>2.90817056881E-2</v>
-      </c>
-      <c r="L15" s="2">
+      <c r="E15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="12">
+        <v>9.2543191189700007</v>
+      </c>
+      <c r="G15" s="12">
+        <v>9.8652577736799998</v>
+      </c>
+      <c r="H15" s="12">
+        <v>6.9642893628399998</v>
+      </c>
+      <c r="I15" s="12">
+        <v>9.2794667252699998</v>
+      </c>
+      <c r="J15" s="12">
+        <v>8.3590643346399993</v>
+      </c>
+      <c r="K15" s="12">
+        <v>5.5978571627299996</v>
+      </c>
+      <c r="L15" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3939,28 +4206,28 @@
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0.29672347742299998</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0.34352575119200002</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0.27507469604200002</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0.29752979122000001</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0.268018706238</v>
-      </c>
-      <c r="K16" s="2">
-        <v>0.17948545128900001</v>
-      </c>
-      <c r="L16" s="2">
+      <c r="E16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="12">
+        <v>4.80775727459E-2</v>
+      </c>
+      <c r="G16" s="12">
+        <v>6.3433137419000002E-2</v>
+      </c>
+      <c r="H16" s="12">
+        <v>5.8545778175500003E-2</v>
+      </c>
+      <c r="I16" s="12">
+        <v>4.8208218323999998E-2</v>
+      </c>
+      <c r="J16" s="12">
+        <v>4.3426590165000001E-2</v>
+      </c>
+      <c r="K16" s="12">
+        <v>2.90817056881E-2</v>
+      </c>
+      <c r="L16" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3969,28 +4236,28 @@
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="2">
-        <v>6.5711996053400001E-3</v>
-      </c>
-      <c r="G17" s="2">
-        <v>1.28864026725E-2</v>
-      </c>
-      <c r="H17" s="2">
-        <v>1.5636813599300001E-2</v>
-      </c>
-      <c r="I17" s="2">
-        <v>6.5890561260100004E-3</v>
-      </c>
-      <c r="J17" s="2">
-        <v>5.9355074696099998E-3</v>
-      </c>
-      <c r="K17" s="2">
-        <v>3.9748615004099996E-3</v>
-      </c>
-      <c r="L17" s="2">
+      <c r="E17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="12">
+        <v>0.29672347742299998</v>
+      </c>
+      <c r="G17" s="12">
+        <v>0.34352575119200002</v>
+      </c>
+      <c r="H17" s="12">
+        <v>0.27507469604200002</v>
+      </c>
+      <c r="I17" s="12">
+        <v>0.29752979122000001</v>
+      </c>
+      <c r="J17" s="12">
+        <v>0.268018706238</v>
+      </c>
+      <c r="K17" s="12">
+        <v>0.17948545128900001</v>
+      </c>
+      <c r="L17" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3999,28 +4266,28 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="2">
-        <v>2.3028684184800001</v>
-      </c>
-      <c r="G18" s="2">
-        <v>2.4299862392999998</v>
-      </c>
-      <c r="H18" s="2">
-        <v>1.7465594236099999</v>
-      </c>
-      <c r="I18" s="2">
-        <v>2.3091262130999999</v>
-      </c>
-      <c r="J18" s="2">
-        <v>2.0800909301699999</v>
-      </c>
-      <c r="K18" s="2">
-        <v>1.3929850814</v>
-      </c>
-      <c r="L18" s="2">
+      <c r="E18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="12">
+        <v>6.5711996053400001E-3</v>
+      </c>
+      <c r="G18" s="12">
+        <v>1.28864026725E-2</v>
+      </c>
+      <c r="H18" s="12">
+        <v>1.5636813599300001E-2</v>
+      </c>
+      <c r="I18" s="12">
+        <v>6.5890561260100004E-3</v>
+      </c>
+      <c r="J18" s="12">
+        <v>5.9355074696099998E-3</v>
+      </c>
+      <c r="K18" s="12">
+        <v>3.9748615004099996E-3</v>
+      </c>
+      <c r="L18" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4029,28 +4296,28 @@
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0.44992271947099999</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0.47315242509599997</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0.36651470944199999</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0.45114533555699998</v>
-      </c>
-      <c r="J19" s="2">
-        <v>0.406397586827</v>
-      </c>
-      <c r="K19" s="2">
-        <v>0.272154340637</v>
-      </c>
-      <c r="L19" s="2">
+      <c r="E19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="12">
+        <v>2.3028684184800001</v>
+      </c>
+      <c r="G19" s="12">
+        <v>2.4299862392999998</v>
+      </c>
+      <c r="H19" s="12">
+        <v>1.7465594236099999</v>
+      </c>
+      <c r="I19" s="12">
+        <v>2.3091262130999999</v>
+      </c>
+      <c r="J19" s="12">
+        <v>2.0800909301699999</v>
+      </c>
+      <c r="K19" s="12">
+        <v>1.3929850814</v>
+      </c>
+      <c r="L19" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4059,28 +4326,28 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1.6640229122500001</v>
-      </c>
-      <c r="G20" s="2">
-        <v>1.74993713869</v>
-      </c>
-      <c r="H20" s="2">
-        <v>1.2782121900900001</v>
-      </c>
-      <c r="I20" s="2">
-        <v>1.66854471364</v>
-      </c>
-      <c r="J20" s="2">
-        <v>1.50304678269</v>
-      </c>
-      <c r="K20" s="2">
-        <v>1.0065529898500001</v>
-      </c>
-      <c r="L20" s="2">
+      <c r="E20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0.44992271947099999</v>
+      </c>
+      <c r="G20" s="12">
+        <v>0.47315242509599997</v>
+      </c>
+      <c r="H20" s="12">
+        <v>0.36651470944199999</v>
+      </c>
+      <c r="I20" s="12">
+        <v>0.45114533555699998</v>
+      </c>
+      <c r="J20" s="12">
+        <v>0.406397586827</v>
+      </c>
+      <c r="K20" s="12">
+        <v>0.272154340637</v>
+      </c>
+      <c r="L20" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4089,28 +4356,28 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="2">
-        <v>14.137242987300001</v>
-      </c>
-      <c r="G21" s="2">
-        <v>15.092160481400001</v>
-      </c>
-      <c r="H21" s="2">
-        <v>10.7023041251</v>
-      </c>
-      <c r="I21" s="2">
-        <v>14.1756594085</v>
-      </c>
-      <c r="J21" s="2">
-        <v>12.769618394</v>
-      </c>
-      <c r="K21" s="2">
-        <v>8.5514953504700006</v>
-      </c>
-      <c r="L21" s="2">
+      <c r="E21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="12">
+        <v>1.6640229122500001</v>
+      </c>
+      <c r="G21" s="12">
+        <v>1.74993713869</v>
+      </c>
+      <c r="H21" s="12">
+        <v>1.2782121900900001</v>
+      </c>
+      <c r="I21" s="12">
+        <v>1.66854471364</v>
+      </c>
+      <c r="J21" s="12">
+        <v>1.50304678269</v>
+      </c>
+      <c r="K21" s="12">
+        <v>1.0065529898500001</v>
+      </c>
+      <c r="L21" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4119,28 +4386,28 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="2">
-        <v>3.36500166636</v>
-      </c>
-      <c r="G22" s="2">
-        <v>3.6631059923099998</v>
-      </c>
-      <c r="H22" s="2">
-        <v>2.6834752969500002</v>
-      </c>
-      <c r="I22" s="2">
-        <v>3.37414569263</v>
-      </c>
-      <c r="J22" s="2">
-        <v>3.0394743312500001</v>
-      </c>
-      <c r="K22" s="2">
-        <v>2.0354602471000001</v>
-      </c>
-      <c r="L22" s="2">
+      <c r="E22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="12">
+        <v>14.137242987300001</v>
+      </c>
+      <c r="G22" s="12">
+        <v>15.092160481400001</v>
+      </c>
+      <c r="H22" s="12">
+        <v>10.7023041251</v>
+      </c>
+      <c r="I22" s="12">
+        <v>14.1756594085</v>
+      </c>
+      <c r="J22" s="12">
+        <v>12.769618394</v>
+      </c>
+      <c r="K22" s="12">
+        <v>8.5514953504700006</v>
+      </c>
+      <c r="L22" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4149,28 +4416,28 @@
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" t="s">
-        <v>28</v>
-      </c>
-      <c r="F23" s="2">
-        <v>6.0013167251599997E-2</v>
-      </c>
-      <c r="G23" s="2">
-        <v>6.7541364618300001E-2</v>
-      </c>
-      <c r="H23" s="2">
-        <v>5.4302857822399998E-2</v>
-      </c>
-      <c r="I23" s="2">
-        <v>6.0176246510400003E-2</v>
-      </c>
-      <c r="J23" s="2">
-        <v>5.4207545636999997E-2</v>
-      </c>
-      <c r="K23" s="2">
-        <v>3.6301443016800002E-2</v>
-      </c>
-      <c r="L23" s="2">
+      <c r="E23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="12">
+        <v>3.36500166636</v>
+      </c>
+      <c r="G23" s="12">
+        <v>3.6631059923099998</v>
+      </c>
+      <c r="H23" s="12">
+        <v>2.6834752969500002</v>
+      </c>
+      <c r="I23" s="12">
+        <v>3.37414569263</v>
+      </c>
+      <c r="J23" s="12">
+        <v>3.0394743312500001</v>
+      </c>
+      <c r="K23" s="12">
+        <v>2.0354602471000001</v>
+      </c>
+      <c r="L23" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4179,28 +4446,28 @@
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="2">
-        <v>0.107099039398</v>
-      </c>
-      <c r="G24" s="2">
-        <v>0.131094554058</v>
-      </c>
-      <c r="H24" s="2">
-        <v>0.112665019182</v>
-      </c>
-      <c r="I24" s="2">
-        <v>0.107390069396</v>
-      </c>
-      <c r="J24" s="2">
-        <v>9.6738371456000005E-2</v>
-      </c>
-      <c r="K24" s="2">
-        <v>6.4783277635700007E-2</v>
-      </c>
-      <c r="L24" s="2">
+      <c r="E24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="12">
+        <v>6.0013167251599997E-2</v>
+      </c>
+      <c r="G24" s="12">
+        <v>6.7541364618300001E-2</v>
+      </c>
+      <c r="H24" s="12">
+        <v>5.4302857822399998E-2</v>
+      </c>
+      <c r="I24" s="12">
+        <v>6.0176246510400003E-2</v>
+      </c>
+      <c r="J24" s="12">
+        <v>5.4207545636999997E-2</v>
+      </c>
+      <c r="K24" s="12">
+        <v>3.6301443016800002E-2</v>
+      </c>
+      <c r="L24" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4209,28 +4476,28 @@
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" s="2">
-        <v>5.8433857149499998E-3</v>
-      </c>
-      <c r="G25" s="2">
-        <v>6.1450822600100001E-3</v>
-      </c>
-      <c r="H25" s="2">
-        <v>8.1418783839599992E-3</v>
-      </c>
-      <c r="I25" s="2">
-        <v>5.8592644804799998E-3</v>
-      </c>
-      <c r="J25" s="2">
-        <v>5.2781016620900003E-3</v>
-      </c>
-      <c r="K25" s="2">
-        <v>3.53461320692E-3</v>
-      </c>
-      <c r="L25" s="2">
+      <c r="E25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="12">
+        <v>0.107099039398</v>
+      </c>
+      <c r="G25" s="12">
+        <v>0.131094554058</v>
+      </c>
+      <c r="H25" s="12">
+        <v>0.112665019182</v>
+      </c>
+      <c r="I25" s="12">
+        <v>0.107390069396</v>
+      </c>
+      <c r="J25" s="12">
+        <v>9.6738371456000005E-2</v>
+      </c>
+      <c r="K25" s="12">
+        <v>6.4783277635700007E-2</v>
+      </c>
+      <c r="L25" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4239,28 +4506,28 @@
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="2">
-        <v>1.04263085165</v>
-      </c>
-      <c r="G26" s="2">
-        <v>1.1296770867599999</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0.82353663306400005</v>
-      </c>
-      <c r="I26" s="2">
-        <v>1.0454640876600001</v>
-      </c>
-      <c r="J26" s="2">
-        <v>0.94176764969899995</v>
-      </c>
-      <c r="K26" s="2">
-        <v>0.63067833580900001</v>
-      </c>
-      <c r="L26" s="2">
+      <c r="E26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="12">
+        <v>5.8433857149499998E-3</v>
+      </c>
+      <c r="G26" s="12">
+        <v>6.1450822600100001E-3</v>
+      </c>
+      <c r="H26" s="12">
+        <v>8.1418783839599992E-3</v>
+      </c>
+      <c r="I26" s="12">
+        <v>5.8592644804799998E-3</v>
+      </c>
+      <c r="J26" s="12">
+        <v>5.2781016620900003E-3</v>
+      </c>
+      <c r="K26" s="12">
+        <v>3.53461320692E-3</v>
+      </c>
+      <c r="L26" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4269,28 +4536,28 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" t="s">
-        <v>32</v>
-      </c>
-      <c r="F27" s="2">
-        <v>14.422518612899999</v>
-      </c>
-      <c r="G27" s="2">
-        <v>15.317941838199999</v>
-      </c>
-      <c r="H27" s="2">
-        <v>10.750998150999999</v>
-      </c>
-      <c r="I27" s="2">
-        <v>14.4617102395</v>
-      </c>
-      <c r="J27" s="2">
-        <v>13.027296703599999</v>
-      </c>
-      <c r="K27" s="2">
-        <v>8.72405609572</v>
-      </c>
-      <c r="L27" s="2">
+      <c r="E27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="12">
+        <v>1.04263085165</v>
+      </c>
+      <c r="G27" s="12">
+        <v>1.1296770867599999</v>
+      </c>
+      <c r="H27" s="12">
+        <v>0.82353663306400005</v>
+      </c>
+      <c r="I27" s="12">
+        <v>1.0454640876600001</v>
+      </c>
+      <c r="J27" s="12">
+        <v>0.94176764969899995</v>
+      </c>
+      <c r="K27" s="12">
+        <v>0.63067833580900001</v>
+      </c>
+      <c r="L27" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4299,28 +4566,28 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" t="s">
-        <v>33</v>
-      </c>
-      <c r="F28" s="2">
-        <v>12.916431923099999</v>
-      </c>
-      <c r="G28" s="2">
-        <v>14.0500143575</v>
-      </c>
-      <c r="H28" s="2">
-        <v>10.232726229600001</v>
-      </c>
-      <c r="I28" s="2">
-        <v>12.9515309229</v>
-      </c>
-      <c r="J28" s="2">
-        <v>11.6669075306</v>
-      </c>
-      <c r="K28" s="2">
-        <v>7.8130373535100004</v>
-      </c>
-      <c r="L28" s="2">
+      <c r="E28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="12">
+        <v>14.422518612899999</v>
+      </c>
+      <c r="G28" s="12">
+        <v>15.317941838199999</v>
+      </c>
+      <c r="H28" s="12">
+        <v>10.750998150999999</v>
+      </c>
+      <c r="I28" s="12">
+        <v>14.4617102395</v>
+      </c>
+      <c r="J28" s="12">
+        <v>13.027296703599999</v>
+      </c>
+      <c r="K28" s="12">
+        <v>8.72405609572</v>
+      </c>
+      <c r="L28" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4329,65 +4596,102 @@
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F29" s="2">
-        <v>4.7495701723800003</v>
-      </c>
-      <c r="G29" s="2">
-        <v>4.9947925454200002</v>
-      </c>
-      <c r="H29" s="2">
-        <v>3.4724035880300002</v>
-      </c>
-      <c r="I29" s="2">
-        <v>4.7624766130699996</v>
-      </c>
-      <c r="J29" s="2">
-        <v>4.2901008839700001</v>
-      </c>
-      <c r="K29" s="2">
-        <v>2.8729736966699999</v>
-      </c>
-      <c r="L29" s="2">
+      <c r="E29" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="12">
+        <v>12.916431923099999</v>
+      </c>
+      <c r="G29" s="12">
+        <v>14.0500143575</v>
+      </c>
+      <c r="H29" s="12">
+        <v>10.232726229600001</v>
+      </c>
+      <c r="I29" s="12">
+        <v>12.9515309229</v>
+      </c>
+      <c r="J29" s="12">
+        <v>11.6669075306</v>
+      </c>
+      <c r="K29" s="12">
+        <v>7.8130373535100004</v>
+      </c>
+      <c r="L29" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E30" s="3" t="s">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="12">
+        <v>4.7495701723800003</v>
+      </c>
+      <c r="G30" s="12">
+        <v>4.9947925454200002</v>
+      </c>
+      <c r="H30" s="12">
+        <v>3.4724035880300002</v>
+      </c>
+      <c r="I30" s="12">
+        <v>4.7624766130699996</v>
+      </c>
+      <c r="J30" s="12">
+        <v>4.2901008839700001</v>
+      </c>
+      <c r="K30" s="12">
+        <v>2.8729736966699999</v>
+      </c>
+      <c r="L30" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E31" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="4">
-        <f>SUM(F3:F29)</f>
+      <c r="F31" s="13">
+        <f>SUM(F4:F30)</f>
         <v>88.169365739178801</v>
       </c>
-      <c r="G30" s="4">
-        <f t="shared" ref="G30:L30" si="0">SUM(G3:G29)</f>
+      <c r="G31" s="13">
+        <f t="shared" ref="G31:L31" si="0">SUM(G4:G30)</f>
         <v>94.188889031281207</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H31" s="13">
         <f t="shared" si="0"/>
         <v>67.176138840456758</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I31" s="13">
         <f t="shared" si="0"/>
         <v>88.408956406948619</v>
       </c>
-      <c r="J30" s="4">
+      <c r="J31" s="13">
         <f t="shared" si="0"/>
         <v>79.639937966672605</v>
       </c>
-      <c r="K30" s="4">
+      <c r="K31" s="13">
         <f t="shared" si="0"/>
         <v>53.332882645518922</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L31" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="3"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="E2:E3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>